<commit_message>
Updated code list mvaSpesifikasjon.xml and prototype example.
Signed-off-by: Lie <Kristian.Lie@skatteetaten.no>
</commit_message>
<xml_diff>
--- a/docs/documentation/test/Testtilfeller mva-melding.xlsx
+++ b/docs/documentation/test/Testtilfeller mva-melding.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20064" windowHeight="6828" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20064" windowHeight="6828" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Testtilfeller" sheetId="4" r:id="rId1"/>
@@ -52,7 +52,6 @@
     <definedName name="_xlnm.Extract" localSheetId="2">'Hjelpeark, ikke bruk'!$B$220</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37650,7 +37649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -39497,8 +39496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD58"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42740,12 +42739,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100771C32DEAFFE3B4B96D01FE0FE913B3B" ma:contentTypeVersion="20" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="aede315d5b925a07e5cacaa0ceea4b20">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8f3bf5a6-5369-4277-b2f1-c47066d1c7ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8002682317f967cbab1e2c1a7ba68677" ns2:_="">
     <xsd:import namespace="8f3bf5a6-5369-4277-b2f1-c47066d1c7ce"/>
@@ -42893,28 +42886,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CFCAF3D-F7CA-43A7-9D83-D55F559FF08A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8f3bf5a6-5369-4277-b2f1-c47066d1c7ce"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36D7E8F5-B790-4687-B69F-6890A7554A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42932,6 +42915,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CFCAF3D-F7CA-43A7-9D83-D55F559FF08A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8f3bf5a6-5369-4277-b2f1-c47066d1c7ce"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E337DF8-E3C2-4E4A-95E3-036EA908DE2B}">
   <ds:schemaRefs>

</xml_diff>